<commit_message>
comptiq years 88 and 89
</commit_message>
<xml_diff>
--- a/comptiq/checklist.xlsx
+++ b/comptiq/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/comptiq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DC55CD-2E0E-8F40-887E-A1B393263680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FFE9C0-83B8-DE43-B1FC-34D5952ED254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{6A734755-0472-A246-937B-814011631BB2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
   <si>
     <t>year</t>
   </si>
@@ -156,6 +156,78 @@
   </si>
   <si>
     <t>1983.jpg</t>
+  </si>
+  <si>
+    <t>1988/01</t>
+  </si>
+  <si>
+    <t>1988/02</t>
+  </si>
+  <si>
+    <t>1988/03</t>
+  </si>
+  <si>
+    <t>1988/04</t>
+  </si>
+  <si>
+    <t>1988/05</t>
+  </si>
+  <si>
+    <t>1988/06</t>
+  </si>
+  <si>
+    <t>1988/07</t>
+  </si>
+  <si>
+    <t>1988/08</t>
+  </si>
+  <si>
+    <t>1988/09</t>
+  </si>
+  <si>
+    <t>1988/10</t>
+  </si>
+  <si>
+    <t>1988/11</t>
+  </si>
+  <si>
+    <t>1988/12</t>
+  </si>
+  <si>
+    <t>1989/01</t>
+  </si>
+  <si>
+    <t>1989/02</t>
+  </si>
+  <si>
+    <t>1989/03</t>
+  </si>
+  <si>
+    <t>1989/04</t>
+  </si>
+  <si>
+    <t>1989/05</t>
+  </si>
+  <si>
+    <t>1989/06</t>
+  </si>
+  <si>
+    <t>1989/07</t>
+  </si>
+  <si>
+    <t>1989/08</t>
+  </si>
+  <si>
+    <t>1989/09</t>
+  </si>
+  <si>
+    <t>1989/10</t>
+  </si>
+  <si>
+    <t>1989/11</t>
+  </si>
+  <si>
+    <t>1989/12</t>
   </si>
 </sst>
 </file>
@@ -523,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83F7A66-A304-A041-AEDA-FBBD35392350}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E49" sqref="E49:E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,7 +666,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="str">
-        <f t="shared" ref="E4:E36" si="0">CONCATENATE(SUBSTITUTE(B4,"/",""), ".jpg")</f>
+        <f t="shared" ref="E4:E60" si="0">CONCATENATE(SUBSTITUTE(B4,"/",""), ".jpg")</f>
         <v>198407.jpg</v>
       </c>
     </row>
@@ -1088,6 +1160,366 @@
       <c r="E36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>198712.jpg</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1988</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198801.jpg</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1988</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198802.jpg</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1988</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198803.jpg</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1988</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198804.jpg</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1988</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198805.jpg</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1988</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198806.jpg</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1988</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198807.jpg</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1988</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198808.jpg</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1988</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198809.jpg</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1988</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198810.jpg</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1988</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198811.jpg</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1988</v>
+      </c>
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198812.jpg</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1989</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198901.jpg</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1989</v>
+      </c>
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198902.jpg</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1989</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198903.jpg</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1989</v>
+      </c>
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198904.jpg</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1989</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198905.jpg</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1989</v>
+      </c>
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198906.jpg</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1989</v>
+      </c>
+      <c r="B55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198907.jpg</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1989</v>
+      </c>
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198908.jpg</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1989</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198909.jpg</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1989</v>
+      </c>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198910.jpg</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1989</v>
+      </c>
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198911.jpg</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1989</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>198912.jpg</v>
       </c>
     </row>
   </sheetData>

</xml_diff>